<commit_message>
v0.2.3 add UTF32 w/o BOM and ValidUtf8
</commit_message>
<xml_diff>
--- a/char_frac.xlsx
+++ b/char_frac.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\gd\=x=\go\src\github.com\softlandia\cpd\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\go\src\github.com\softlandia\cpd\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="170">
   <si>
     <t>,</t>
   </si>
@@ -995,7 +995,7 @@
   <dimension ref="A1:M35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="H17" sqref="H17:I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1444,11 +1444,17 @@
       <c r="G14" s="14">
         <v>3.2099999999999997E-2</v>
       </c>
-      <c r="H14" s="4" t="s">
+      <c r="H14" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="I14" s="4" t="s">
+      <c r="I14" s="6" t="s">
         <v>40</v>
+      </c>
+      <c r="J14" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="K14" s="9" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -1471,11 +1477,17 @@
       <c r="G15" s="14">
         <v>2.98E-2</v>
       </c>
-      <c r="H15" s="4" t="s">
+      <c r="H15" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="I15" s="4" t="s">
+      <c r="I15" s="6" t="s">
         <v>78</v>
+      </c>
+      <c r="J15" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="K15" s="11" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -1498,14 +1510,20 @@
       <c r="G16" s="14">
         <v>2.81E-2</v>
       </c>
-      <c r="H16" s="4" t="s">
+      <c r="H16" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="I16" s="4" t="s">
+      <c r="I16" s="6" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J16" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="K16" s="11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>15</v>
       </c>
@@ -1525,14 +1543,20 @@
       <c r="G17" s="14">
         <v>2.6200000000000001E-2</v>
       </c>
-      <c r="H17" s="4" t="s">
+      <c r="H17" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="I17" s="4" t="s">
+      <c r="I17" s="7" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J17" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="K17" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>16</v>
       </c>
@@ -1559,7 +1583,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>17</v>
       </c>
@@ -1586,7 +1610,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>18</v>
       </c>
@@ -1613,7 +1637,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>19</v>
       </c>
@@ -1640,7 +1664,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>20</v>
       </c>
@@ -1667,7 +1691,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>21</v>
       </c>
@@ -1694,7 +1718,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>22</v>
       </c>
@@ -1721,7 +1745,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>23</v>
       </c>
@@ -1748,7 +1772,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>24</v>
       </c>
@@ -1775,7 +1799,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>25</v>
       </c>
@@ -1802,7 +1826,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>26</v>
       </c>
@@ -1829,7 +1853,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>27</v>
       </c>
@@ -1856,7 +1880,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>28</v>
       </c>
@@ -1883,7 +1907,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>29</v>
       </c>
@@ -1910,7 +1934,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>30</v>
       </c>

</xml_diff>